<commit_message>
change the sample, Because the "関数" sheet is displayed firs、
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="240" documentId="13_ncr:1_{A00D83F5-B591-4B8C-A3D9-0A7E1F129DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C58A8E9A-7691-47F1-BE89-6BB5E9400D61}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="1050" windowWidth="21600" windowHeight="13890" activeTab="1" xr2:uid="{F6454EEB-C728-456F-9F74-DCB3B1160FD6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F6454EEB-C728-456F-9F74-DCB3B1160FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="基本" sheetId="3" r:id="rId1"/>
@@ -3529,9 +3529,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3542,6 +3539,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5781,7 +5781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7795CA75-2E57-4007-A1E6-AF0752BF2C5D}">
   <dimension ref="B2:B20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -6444,258 +6444,258 @@
       <c r="B5" s="109" t="s">
         <v>216</v>
       </c>
-      <c r="C5" s="112">
+      <c r="C5" s="111">
         <v>1</v>
       </c>
-      <c r="D5" s="113"/>
-      <c r="E5" s="112">
+      <c r="D5" s="112"/>
+      <c r="E5" s="111">
         <v>2</v>
       </c>
-      <c r="F5" s="113"/>
-      <c r="G5" s="112">
+      <c r="F5" s="112"/>
+      <c r="G5" s="111">
         <v>3</v>
       </c>
-      <c r="H5" s="113"/>
-      <c r="I5" s="112">
+      <c r="H5" s="112"/>
+      <c r="I5" s="111">
         <v>4</v>
       </c>
-      <c r="J5" s="113"/>
-      <c r="K5" s="114">
+      <c r="J5" s="112"/>
+      <c r="K5" s="113">
         <v>5</v>
       </c>
-      <c r="L5" s="115"/>
-      <c r="M5" s="114">
+      <c r="L5" s="114"/>
+      <c r="M5" s="113">
         <v>6</v>
       </c>
-      <c r="N5" s="115"/>
-      <c r="O5" s="112">
+      <c r="N5" s="114"/>
+      <c r="O5" s="111">
         <v>7</v>
       </c>
-      <c r="P5" s="113"/>
-      <c r="Q5" s="112">
+      <c r="P5" s="112"/>
+      <c r="Q5" s="111">
         <v>8</v>
       </c>
-      <c r="R5" s="113"/>
-      <c r="S5" s="112">
+      <c r="R5" s="112"/>
+      <c r="S5" s="111">
         <v>9</v>
       </c>
-      <c r="T5" s="113"/>
-      <c r="U5" s="112">
+      <c r="T5" s="112"/>
+      <c r="U5" s="111">
         <v>10</v>
       </c>
-      <c r="V5" s="113"/>
-      <c r="W5" s="112">
+      <c r="V5" s="112"/>
+      <c r="W5" s="111">
         <v>11</v>
       </c>
-      <c r="X5" s="113"/>
-      <c r="Y5" s="114">
+      <c r="X5" s="112"/>
+      <c r="Y5" s="113">
         <v>12</v>
       </c>
-      <c r="Z5" s="115"/>
-      <c r="AA5" s="114">
+      <c r="Z5" s="114"/>
+      <c r="AA5" s="113">
         <v>13</v>
       </c>
-      <c r="AB5" s="115"/>
-      <c r="AC5" s="112">
+      <c r="AB5" s="114"/>
+      <c r="AC5" s="111">
         <v>14</v>
       </c>
-      <c r="AD5" s="113"/>
-      <c r="AE5" s="112">
+      <c r="AD5" s="112"/>
+      <c r="AE5" s="111">
         <v>15</v>
       </c>
-      <c r="AF5" s="113"/>
-      <c r="AG5" s="112">
+      <c r="AF5" s="112"/>
+      <c r="AG5" s="111">
         <v>16</v>
       </c>
-      <c r="AH5" s="113"/>
-      <c r="AI5" s="112">
+      <c r="AH5" s="112"/>
+      <c r="AI5" s="111">
         <v>17</v>
       </c>
-      <c r="AJ5" s="113"/>
-      <c r="AK5" s="112">
+      <c r="AJ5" s="112"/>
+      <c r="AK5" s="111">
         <v>18</v>
       </c>
-      <c r="AL5" s="113"/>
-      <c r="AM5" s="114">
+      <c r="AL5" s="112"/>
+      <c r="AM5" s="113">
         <v>19</v>
       </c>
-      <c r="AN5" s="115"/>
-      <c r="AO5" s="114">
+      <c r="AN5" s="114"/>
+      <c r="AO5" s="113">
         <v>20</v>
       </c>
-      <c r="AP5" s="115"/>
-      <c r="AQ5" s="112">
+      <c r="AP5" s="114"/>
+      <c r="AQ5" s="111">
         <v>21</v>
       </c>
-      <c r="AR5" s="113"/>
-      <c r="AS5" s="112">
+      <c r="AR5" s="112"/>
+      <c r="AS5" s="111">
         <v>22</v>
       </c>
-      <c r="AT5" s="113"/>
-      <c r="AU5" s="112">
+      <c r="AT5" s="112"/>
+      <c r="AU5" s="111">
         <v>23</v>
       </c>
-      <c r="AV5" s="113"/>
-      <c r="AW5" s="112">
+      <c r="AV5" s="112"/>
+      <c r="AW5" s="111">
         <v>24</v>
       </c>
-      <c r="AX5" s="113"/>
-      <c r="AY5" s="112">
+      <c r="AX5" s="112"/>
+      <c r="AY5" s="111">
         <v>25</v>
       </c>
-      <c r="AZ5" s="113"/>
-      <c r="BA5" s="114">
+      <c r="AZ5" s="112"/>
+      <c r="BA5" s="113">
         <v>26</v>
       </c>
-      <c r="BB5" s="115"/>
-      <c r="BC5" s="114">
+      <c r="BB5" s="114"/>
+      <c r="BC5" s="113">
         <v>27</v>
       </c>
-      <c r="BD5" s="115"/>
-      <c r="BE5" s="112">
+      <c r="BD5" s="114"/>
+      <c r="BE5" s="111">
         <v>28</v>
       </c>
-      <c r="BF5" s="113"/>
-      <c r="BG5" s="112">
+      <c r="BF5" s="112"/>
+      <c r="BG5" s="111">
         <v>29</v>
       </c>
-      <c r="BH5" s="113"/>
-      <c r="BI5" s="112">
+      <c r="BH5" s="112"/>
+      <c r="BI5" s="111">
         <v>30</v>
       </c>
-      <c r="BJ5" s="113"/>
-      <c r="BK5" s="112">
+      <c r="BJ5" s="112"/>
+      <c r="BK5" s="111">
         <v>31</v>
       </c>
-      <c r="BL5" s="113"/>
+      <c r="BL5" s="112"/>
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.4">
-      <c r="A6" s="111"/>
-      <c r="B6" s="111"/>
-      <c r="C6" s="112" t="s">
+      <c r="A6" s="115"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="111" t="s">
         <v>217</v>
       </c>
-      <c r="D6" s="113"/>
-      <c r="E6" s="112" t="s">
+      <c r="D6" s="112"/>
+      <c r="E6" s="111" t="s">
         <v>218</v>
       </c>
-      <c r="F6" s="113"/>
-      <c r="G6" s="112" t="s">
+      <c r="F6" s="112"/>
+      <c r="G6" s="111" t="s">
         <v>258</v>
       </c>
-      <c r="H6" s="113"/>
-      <c r="I6" s="112" t="s">
+      <c r="H6" s="112"/>
+      <c r="I6" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="J6" s="113"/>
-      <c r="K6" s="114" t="s">
+      <c r="J6" s="112"/>
+      <c r="K6" s="113" t="s">
         <v>263</v>
       </c>
-      <c r="L6" s="115"/>
-      <c r="M6" s="114" t="s">
+      <c r="L6" s="114"/>
+      <c r="M6" s="113" t="s">
         <v>262</v>
       </c>
-      <c r="N6" s="115"/>
-      <c r="O6" s="112" t="s">
+      <c r="N6" s="114"/>
+      <c r="O6" s="111" t="s">
         <v>261</v>
       </c>
-      <c r="P6" s="113"/>
-      <c r="Q6" s="112" t="s">
+      <c r="P6" s="112"/>
+      <c r="Q6" s="111" t="s">
         <v>260</v>
       </c>
-      <c r="R6" s="113"/>
-      <c r="S6" s="112" t="s">
+      <c r="R6" s="112"/>
+      <c r="S6" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="T6" s="113"/>
-      <c r="U6" s="112" t="s">
+      <c r="T6" s="112"/>
+      <c r="U6" s="111" t="s">
         <v>258</v>
       </c>
-      <c r="V6" s="113"/>
-      <c r="W6" s="112" t="s">
+      <c r="V6" s="112"/>
+      <c r="W6" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="X6" s="113"/>
-      <c r="Y6" s="114" t="s">
+      <c r="X6" s="112"/>
+      <c r="Y6" s="113" t="s">
         <v>263</v>
       </c>
-      <c r="Z6" s="115"/>
-      <c r="AA6" s="114" t="s">
+      <c r="Z6" s="114"/>
+      <c r="AA6" s="113" t="s">
         <v>262</v>
       </c>
-      <c r="AB6" s="115"/>
-      <c r="AC6" s="112" t="s">
+      <c r="AB6" s="114"/>
+      <c r="AC6" s="111" t="s">
         <v>261</v>
       </c>
-      <c r="AD6" s="113"/>
-      <c r="AE6" s="112" t="s">
+      <c r="AD6" s="112"/>
+      <c r="AE6" s="111" t="s">
         <v>260</v>
       </c>
-      <c r="AF6" s="113"/>
-      <c r="AG6" s="112" t="s">
+      <c r="AF6" s="112"/>
+      <c r="AG6" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="AH6" s="113"/>
-      <c r="AI6" s="112" t="s">
+      <c r="AH6" s="112"/>
+      <c r="AI6" s="111" t="s">
         <v>258</v>
       </c>
-      <c r="AJ6" s="113"/>
-      <c r="AK6" s="112" t="s">
+      <c r="AJ6" s="112"/>
+      <c r="AK6" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="AL6" s="113"/>
-      <c r="AM6" s="114" t="s">
+      <c r="AL6" s="112"/>
+      <c r="AM6" s="113" t="s">
         <v>263</v>
       </c>
-      <c r="AN6" s="115"/>
-      <c r="AO6" s="114" t="s">
+      <c r="AN6" s="114"/>
+      <c r="AO6" s="113" t="s">
         <v>262</v>
       </c>
-      <c r="AP6" s="115"/>
-      <c r="AQ6" s="112" t="s">
+      <c r="AP6" s="114"/>
+      <c r="AQ6" s="111" t="s">
         <v>261</v>
       </c>
-      <c r="AR6" s="113"/>
-      <c r="AS6" s="112" t="s">
+      <c r="AR6" s="112"/>
+      <c r="AS6" s="111" t="s">
         <v>260</v>
       </c>
-      <c r="AT6" s="113"/>
-      <c r="AU6" s="112" t="s">
+      <c r="AT6" s="112"/>
+      <c r="AU6" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="AV6" s="113"/>
-      <c r="AW6" s="112" t="s">
+      <c r="AV6" s="112"/>
+      <c r="AW6" s="111" t="s">
         <v>258</v>
       </c>
-      <c r="AX6" s="113"/>
-      <c r="AY6" s="112" t="s">
+      <c r="AX6" s="112"/>
+      <c r="AY6" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="AZ6" s="113"/>
-      <c r="BA6" s="114" t="s">
+      <c r="AZ6" s="112"/>
+      <c r="BA6" s="113" t="s">
         <v>263</v>
       </c>
-      <c r="BB6" s="115"/>
-      <c r="BC6" s="114" t="s">
+      <c r="BB6" s="114"/>
+      <c r="BC6" s="113" t="s">
         <v>262</v>
       </c>
-      <c r="BD6" s="115"/>
-      <c r="BE6" s="112" t="s">
+      <c r="BD6" s="114"/>
+      <c r="BE6" s="111" t="s">
         <v>261</v>
       </c>
-      <c r="BF6" s="113"/>
-      <c r="BG6" s="112" t="s">
+      <c r="BF6" s="112"/>
+      <c r="BG6" s="111" t="s">
         <v>260</v>
       </c>
-      <c r="BH6" s="113"/>
-      <c r="BI6" s="112" t="s">
+      <c r="BH6" s="112"/>
+      <c r="BI6" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="BJ6" s="113"/>
-      <c r="BK6" s="112" t="s">
+      <c r="BJ6" s="112"/>
+      <c r="BK6" s="111" t="s">
         <v>258</v>
       </c>
-      <c r="BL6" s="113"/>
+      <c r="BL6" s="112"/>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A7" s="110"/>
@@ -7227,54 +7227,6 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="BE6:BF6"/>
-    <mergeCell ref="BG6:BH6"/>
-    <mergeCell ref="BI6:BJ6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="BA6:BB6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BG5:BH5"/>
-    <mergeCell ref="BI5:BJ5"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BE5:BF5"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="AS6:AT6"/>
@@ -7291,6 +7243,54 @@
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="BG5:BH5"/>
+    <mergeCell ref="BI5:BJ5"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BE5:BF5"/>
+    <mergeCell ref="BE6:BF6"/>
+    <mergeCell ref="BG6:BH6"/>
+    <mergeCell ref="BI6:BJ6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="BA6:BB6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AS5:AT5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17064,7 +17064,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -17613,7 +17613,7 @@
     <row r="10" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B10" s="108">
         <f ca="1">RANDBETWEEN(0,2)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" s="90"/>
       <c r="D10" s="91">

</xml_diff>

<commit_message>
delete Functions Exercise 4 of Sample
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://toyotajp-my.sharepoint.com/personal/3169885_tmc_twfr_toyota_co_jp/Documents/01_PA/04_人材育成/01_研修/01_デジタル全員研修/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="240" documentId="13_ncr:1_{A00D83F5-B591-4B8C-A3D9-0A7E1F129DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C58A8E9A-7691-47F1-BE89-6BB5E9400D61}"/>
+  <xr:revisionPtr revIDLastSave="252" documentId="13_ncr:1_{A00D83F5-B591-4B8C-A3D9-0A7E1F129DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEC9916A-AF00-4AB4-9F7C-386AD76F5CF1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F6454EEB-C728-456F-9F74-DCB3B1160FD6}"/>
+    <workbookView xWindow="3135" yWindow="1830" windowWidth="23250" windowHeight="13395" xr2:uid="{F6454EEB-C728-456F-9F74-DCB3B1160FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="基本" sheetId="3" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2951" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2947" uniqueCount="425">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -1641,13 +1641,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>演習7：</t>
-    <rPh sb="0" eb="2">
-      <t>エンシュウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>女性のみの身長・体重の平均値をSUMIF関数、COUNTIF関数を使わずに算出しましょう</t>
     <rPh sb="0" eb="2">
       <t>ジョセイ</t>
@@ -2573,46 +2566,24 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>レコード数と合計を別々に算出して、それを改めて参照するのは面倒ですよね？</t>
-    <rPh sb="4" eb="5">
+    <t>わざわざ合計とレコード数を別に出してから算出するのは面倒ですよね</t>
+    <rPh sb="4" eb="6">
+      <t>ゴウケイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
       <t>スウ</t>
     </rPh>
-    <rPh sb="6" eb="8">
-      <t>ゴウケイ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ベツベツ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
+    <rPh sb="13" eb="14">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
       <t>サンシュツ</t>
     </rPh>
-    <rPh sb="20" eb="21">
-      <t>アラタ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
+    <rPh sb="26" eb="28">
       <t>メンドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SUM関数とCOUNT関数をひとつの式にして、平均値を算出するように数式を変更しましょう</t>
-    <rPh sb="3" eb="5">
-      <t>カンスウ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>カンスウ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>シキ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>スウシキ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>ヘンコウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3529,6 +3500,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3539,9 +3513,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3684,13 +3655,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>338138</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>712518</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>21272</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3734,13 +3705,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>338138</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>712518</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>21272</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3784,7 +3755,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>338138</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="372475" cy="346075"/>
@@ -5842,7 +5813,7 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B20" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -6444,258 +6415,258 @@
       <c r="B5" s="109" t="s">
         <v>216</v>
       </c>
-      <c r="C5" s="111">
+      <c r="C5" s="112">
         <v>1</v>
       </c>
-      <c r="D5" s="112"/>
-      <c r="E5" s="111">
+      <c r="D5" s="113"/>
+      <c r="E5" s="112">
         <v>2</v>
       </c>
-      <c r="F5" s="112"/>
-      <c r="G5" s="111">
+      <c r="F5" s="113"/>
+      <c r="G5" s="112">
         <v>3</v>
       </c>
-      <c r="H5" s="112"/>
-      <c r="I5" s="111">
+      <c r="H5" s="113"/>
+      <c r="I5" s="112">
         <v>4</v>
       </c>
-      <c r="J5" s="112"/>
-      <c r="K5" s="113">
+      <c r="J5" s="113"/>
+      <c r="K5" s="114">
         <v>5</v>
       </c>
-      <c r="L5" s="114"/>
-      <c r="M5" s="113">
+      <c r="L5" s="115"/>
+      <c r="M5" s="114">
         <v>6</v>
       </c>
-      <c r="N5" s="114"/>
-      <c r="O5" s="111">
+      <c r="N5" s="115"/>
+      <c r="O5" s="112">
         <v>7</v>
       </c>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="111">
+      <c r="P5" s="113"/>
+      <c r="Q5" s="112">
         <v>8</v>
       </c>
-      <c r="R5" s="112"/>
-      <c r="S5" s="111">
+      <c r="R5" s="113"/>
+      <c r="S5" s="112">
         <v>9</v>
       </c>
-      <c r="T5" s="112"/>
-      <c r="U5" s="111">
+      <c r="T5" s="113"/>
+      <c r="U5" s="112">
         <v>10</v>
       </c>
-      <c r="V5" s="112"/>
-      <c r="W5" s="111">
+      <c r="V5" s="113"/>
+      <c r="W5" s="112">
         <v>11</v>
       </c>
-      <c r="X5" s="112"/>
-      <c r="Y5" s="113">
+      <c r="X5" s="113"/>
+      <c r="Y5" s="114">
         <v>12</v>
       </c>
-      <c r="Z5" s="114"/>
-      <c r="AA5" s="113">
+      <c r="Z5" s="115"/>
+      <c r="AA5" s="114">
         <v>13</v>
       </c>
-      <c r="AB5" s="114"/>
-      <c r="AC5" s="111">
+      <c r="AB5" s="115"/>
+      <c r="AC5" s="112">
         <v>14</v>
       </c>
-      <c r="AD5" s="112"/>
-      <c r="AE5" s="111">
+      <c r="AD5" s="113"/>
+      <c r="AE5" s="112">
         <v>15</v>
       </c>
-      <c r="AF5" s="112"/>
-      <c r="AG5" s="111">
+      <c r="AF5" s="113"/>
+      <c r="AG5" s="112">
         <v>16</v>
       </c>
-      <c r="AH5" s="112"/>
-      <c r="AI5" s="111">
+      <c r="AH5" s="113"/>
+      <c r="AI5" s="112">
         <v>17</v>
       </c>
-      <c r="AJ5" s="112"/>
-      <c r="AK5" s="111">
+      <c r="AJ5" s="113"/>
+      <c r="AK5" s="112">
         <v>18</v>
       </c>
-      <c r="AL5" s="112"/>
-      <c r="AM5" s="113">
+      <c r="AL5" s="113"/>
+      <c r="AM5" s="114">
         <v>19</v>
       </c>
-      <c r="AN5" s="114"/>
-      <c r="AO5" s="113">
+      <c r="AN5" s="115"/>
+      <c r="AO5" s="114">
         <v>20</v>
       </c>
-      <c r="AP5" s="114"/>
-      <c r="AQ5" s="111">
+      <c r="AP5" s="115"/>
+      <c r="AQ5" s="112">
         <v>21</v>
       </c>
-      <c r="AR5" s="112"/>
-      <c r="AS5" s="111">
+      <c r="AR5" s="113"/>
+      <c r="AS5" s="112">
         <v>22</v>
       </c>
-      <c r="AT5" s="112"/>
-      <c r="AU5" s="111">
+      <c r="AT5" s="113"/>
+      <c r="AU5" s="112">
         <v>23</v>
       </c>
-      <c r="AV5" s="112"/>
-      <c r="AW5" s="111">
+      <c r="AV5" s="113"/>
+      <c r="AW5" s="112">
         <v>24</v>
       </c>
-      <c r="AX5" s="112"/>
-      <c r="AY5" s="111">
+      <c r="AX5" s="113"/>
+      <c r="AY5" s="112">
         <v>25</v>
       </c>
-      <c r="AZ5" s="112"/>
-      <c r="BA5" s="113">
+      <c r="AZ5" s="113"/>
+      <c r="BA5" s="114">
         <v>26</v>
       </c>
-      <c r="BB5" s="114"/>
-      <c r="BC5" s="113">
+      <c r="BB5" s="115"/>
+      <c r="BC5" s="114">
         <v>27</v>
       </c>
-      <c r="BD5" s="114"/>
-      <c r="BE5" s="111">
+      <c r="BD5" s="115"/>
+      <c r="BE5" s="112">
         <v>28</v>
       </c>
-      <c r="BF5" s="112"/>
-      <c r="BG5" s="111">
+      <c r="BF5" s="113"/>
+      <c r="BG5" s="112">
         <v>29</v>
       </c>
-      <c r="BH5" s="112"/>
-      <c r="BI5" s="111">
+      <c r="BH5" s="113"/>
+      <c r="BI5" s="112">
         <v>30</v>
       </c>
-      <c r="BJ5" s="112"/>
-      <c r="BK5" s="111">
+      <c r="BJ5" s="113"/>
+      <c r="BK5" s="112">
         <v>31</v>
       </c>
-      <c r="BL5" s="112"/>
+      <c r="BL5" s="113"/>
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.4">
-      <c r="A6" s="115"/>
-      <c r="B6" s="115"/>
-      <c r="C6" s="111" t="s">
+      <c r="A6" s="111"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="112" t="s">
         <v>217</v>
       </c>
-      <c r="D6" s="112"/>
-      <c r="E6" s="111" t="s">
+      <c r="D6" s="113"/>
+      <c r="E6" s="112" t="s">
         <v>218</v>
       </c>
-      <c r="F6" s="112"/>
-      <c r="G6" s="111" t="s">
+      <c r="F6" s="113"/>
+      <c r="G6" s="112" t="s">
         <v>258</v>
       </c>
-      <c r="H6" s="112"/>
-      <c r="I6" s="111" t="s">
+      <c r="H6" s="113"/>
+      <c r="I6" s="112" t="s">
         <v>264</v>
       </c>
-      <c r="J6" s="112"/>
-      <c r="K6" s="113" t="s">
+      <c r="J6" s="113"/>
+      <c r="K6" s="114" t="s">
         <v>263</v>
       </c>
-      <c r="L6" s="114"/>
-      <c r="M6" s="113" t="s">
+      <c r="L6" s="115"/>
+      <c r="M6" s="114" t="s">
         <v>262</v>
       </c>
-      <c r="N6" s="114"/>
-      <c r="O6" s="111" t="s">
+      <c r="N6" s="115"/>
+      <c r="O6" s="112" t="s">
         <v>261</v>
       </c>
-      <c r="P6" s="112"/>
-      <c r="Q6" s="111" t="s">
+      <c r="P6" s="113"/>
+      <c r="Q6" s="112" t="s">
         <v>260</v>
       </c>
-      <c r="R6" s="112"/>
-      <c r="S6" s="111" t="s">
+      <c r="R6" s="113"/>
+      <c r="S6" s="112" t="s">
         <v>259</v>
       </c>
-      <c r="T6" s="112"/>
-      <c r="U6" s="111" t="s">
+      <c r="T6" s="113"/>
+      <c r="U6" s="112" t="s">
         <v>258</v>
       </c>
-      <c r="V6" s="112"/>
-      <c r="W6" s="111" t="s">
+      <c r="V6" s="113"/>
+      <c r="W6" s="112" t="s">
         <v>264</v>
       </c>
-      <c r="X6" s="112"/>
-      <c r="Y6" s="113" t="s">
+      <c r="X6" s="113"/>
+      <c r="Y6" s="114" t="s">
         <v>263</v>
       </c>
-      <c r="Z6" s="114"/>
-      <c r="AA6" s="113" t="s">
+      <c r="Z6" s="115"/>
+      <c r="AA6" s="114" t="s">
         <v>262</v>
       </c>
-      <c r="AB6" s="114"/>
-      <c r="AC6" s="111" t="s">
+      <c r="AB6" s="115"/>
+      <c r="AC6" s="112" t="s">
         <v>261</v>
       </c>
-      <c r="AD6" s="112"/>
-      <c r="AE6" s="111" t="s">
+      <c r="AD6" s="113"/>
+      <c r="AE6" s="112" t="s">
         <v>260</v>
       </c>
-      <c r="AF6" s="112"/>
-      <c r="AG6" s="111" t="s">
+      <c r="AF6" s="113"/>
+      <c r="AG6" s="112" t="s">
         <v>259</v>
       </c>
-      <c r="AH6" s="112"/>
-      <c r="AI6" s="111" t="s">
+      <c r="AH6" s="113"/>
+      <c r="AI6" s="112" t="s">
         <v>258</v>
       </c>
-      <c r="AJ6" s="112"/>
-      <c r="AK6" s="111" t="s">
+      <c r="AJ6" s="113"/>
+      <c r="AK6" s="112" t="s">
         <v>264</v>
       </c>
-      <c r="AL6" s="112"/>
-      <c r="AM6" s="113" t="s">
+      <c r="AL6" s="113"/>
+      <c r="AM6" s="114" t="s">
         <v>263</v>
       </c>
-      <c r="AN6" s="114"/>
-      <c r="AO6" s="113" t="s">
+      <c r="AN6" s="115"/>
+      <c r="AO6" s="114" t="s">
         <v>262</v>
       </c>
-      <c r="AP6" s="114"/>
-      <c r="AQ6" s="111" t="s">
+      <c r="AP6" s="115"/>
+      <c r="AQ6" s="112" t="s">
         <v>261</v>
       </c>
-      <c r="AR6" s="112"/>
-      <c r="AS6" s="111" t="s">
+      <c r="AR6" s="113"/>
+      <c r="AS6" s="112" t="s">
         <v>260</v>
       </c>
-      <c r="AT6" s="112"/>
-      <c r="AU6" s="111" t="s">
+      <c r="AT6" s="113"/>
+      <c r="AU6" s="112" t="s">
         <v>259</v>
       </c>
-      <c r="AV6" s="112"/>
-      <c r="AW6" s="111" t="s">
+      <c r="AV6" s="113"/>
+      <c r="AW6" s="112" t="s">
         <v>258</v>
       </c>
-      <c r="AX6" s="112"/>
-      <c r="AY6" s="111" t="s">
+      <c r="AX6" s="113"/>
+      <c r="AY6" s="112" t="s">
         <v>264</v>
       </c>
-      <c r="AZ6" s="112"/>
-      <c r="BA6" s="113" t="s">
+      <c r="AZ6" s="113"/>
+      <c r="BA6" s="114" t="s">
         <v>263</v>
       </c>
-      <c r="BB6" s="114"/>
-      <c r="BC6" s="113" t="s">
+      <c r="BB6" s="115"/>
+      <c r="BC6" s="114" t="s">
         <v>262</v>
       </c>
-      <c r="BD6" s="114"/>
-      <c r="BE6" s="111" t="s">
+      <c r="BD6" s="115"/>
+      <c r="BE6" s="112" t="s">
         <v>261</v>
       </c>
-      <c r="BF6" s="112"/>
-      <c r="BG6" s="111" t="s">
+      <c r="BF6" s="113"/>
+      <c r="BG6" s="112" t="s">
         <v>260</v>
       </c>
-      <c r="BH6" s="112"/>
-      <c r="BI6" s="111" t="s">
+      <c r="BH6" s="113"/>
+      <c r="BI6" s="112" t="s">
         <v>259</v>
       </c>
-      <c r="BJ6" s="112"/>
-      <c r="BK6" s="111" t="s">
+      <c r="BJ6" s="113"/>
+      <c r="BK6" s="112" t="s">
         <v>258</v>
       </c>
-      <c r="BL6" s="112"/>
+      <c r="BL6" s="113"/>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A7" s="110"/>
@@ -7227,6 +7198,54 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AS5:AT5"/>
+    <mergeCell ref="BE6:BF6"/>
+    <mergeCell ref="BG6:BH6"/>
+    <mergeCell ref="BI6:BJ6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="BA6:BB6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BG5:BH5"/>
+    <mergeCell ref="BI5:BJ5"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BE5:BF5"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="AS6:AT6"/>
@@ -7243,54 +7262,6 @@
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="BG5:BH5"/>
-    <mergeCell ref="BI5:BJ5"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BE5:BF5"/>
-    <mergeCell ref="BE6:BF6"/>
-    <mergeCell ref="BG6:BH6"/>
-    <mergeCell ref="BI6:BJ6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="BA6:BB6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7314,15 +7285,15 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B2" s="21" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C3" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>307</v>
       </c>
       <c r="F3" s="31"/>
       <c r="G3" s="31"/>
@@ -7331,10 +7302,10 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C4" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>308</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>309</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -7349,10 +7320,10 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E6" t="s">
         <v>310</v>
-      </c>
-      <c r="E6" t="s">
-        <v>311</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -7374,10 +7345,10 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
+        <v>311</v>
+      </c>
+      <c r="E9" t="s">
         <v>312</v>
-      </c>
-      <c r="E9" t="s">
-        <v>313</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -7399,10 +7370,10 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D12" t="s">
+        <v>313</v>
+      </c>
+      <c r="E12" t="s">
         <v>314</v>
-      </c>
-      <c r="E12" t="s">
-        <v>315</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -7424,10 +7395,10 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
+        <v>315</v>
+      </c>
+      <c r="E15" t="s">
         <v>316</v>
-      </c>
-      <c r="E15" t="s">
-        <v>317</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -7449,10 +7420,10 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D18" t="s">
+        <v>317</v>
+      </c>
+      <c r="E18" t="s">
         <v>318</v>
-      </c>
-      <c r="E18" t="s">
-        <v>319</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -7474,15 +7445,15 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B22" s="21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C23" t="s">
+        <v>320</v>
+      </c>
+      <c r="D23" t="s">
         <v>321</v>
-      </c>
-      <c r="D23" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.4">
@@ -7495,10 +7466,10 @@
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D26" t="s">
+        <v>322</v>
+      </c>
+      <c r="E26" t="s">
         <v>323</v>
-      </c>
-      <c r="E26" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.4">
@@ -7506,10 +7477,10 @@
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D29" t="s">
+        <v>324</v>
+      </c>
+      <c r="E29" t="s">
         <v>325</v>
-      </c>
-      <c r="E29" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.4">
@@ -7517,13 +7488,13 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B32" s="21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B33" s="21"/>
       <c r="C33" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.4">
@@ -7533,10 +7504,10 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.4">
       <c r="D35" t="s">
+        <v>328</v>
+      </c>
+      <c r="E35" t="s">
         <v>329</v>
-      </c>
-      <c r="E35" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.4">
@@ -7544,20 +7515,20 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C37" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="38" spans="2:13" ht="37.5" x14ac:dyDescent="0.4">
       <c r="C38" s="39" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.4">
       <c r="D39" t="s">
+        <v>332</v>
+      </c>
+      <c r="E39" t="s">
         <v>333</v>
-      </c>
-      <c r="E39" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.4">
@@ -7565,48 +7536,48 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B42" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="M42" s="41" t="s">
         <v>335</v>
-      </c>
-      <c r="M42" s="41" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C43" s="42"/>
       <c r="D43" s="43" t="s">
+        <v>336</v>
+      </c>
+      <c r="E43" s="43" t="s">
         <v>337</v>
       </c>
-      <c r="E43" s="43" t="s">
+      <c r="F43" s="43" t="s">
         <v>338</v>
       </c>
-      <c r="F43" s="43" t="s">
+      <c r="G43" s="44" t="s">
         <v>339</v>
       </c>
-      <c r="G43" s="44" t="s">
+      <c r="H43" s="45" t="s">
         <v>340</v>
       </c>
-      <c r="H43" s="45" t="s">
+      <c r="I43" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="I43" s="46" t="s">
+      <c r="J43" s="47" t="s">
         <v>342</v>
       </c>
-      <c r="J43" s="47" t="s">
+      <c r="K43" s="48" t="s">
         <v>343</v>
       </c>
-      <c r="K43" s="48" t="s">
+      <c r="L43" s="43" t="s">
         <v>344</v>
       </c>
-      <c r="L43" s="43" t="s">
+      <c r="M43" s="43" t="s">
         <v>345</v>
-      </c>
-      <c r="M43" s="43" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C44" s="49" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D44" s="50">
         <v>371920</v>
@@ -7641,7 +7612,7 @@
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C45" s="49" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D45" s="50">
         <v>384654</v>
@@ -7676,7 +7647,7 @@
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C46" s="49" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D46" s="50">
         <v>117884</v>
@@ -7711,7 +7682,7 @@
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C47" s="49" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D47" s="50">
         <v>72458</v>
@@ -7746,7 +7717,7 @@
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C48" s="49" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D48" s="50">
         <v>153834</v>
@@ -7781,7 +7752,7 @@
     </row>
     <row r="49" spans="3:13" x14ac:dyDescent="0.4">
       <c r="C49" s="49" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D49" s="50">
         <v>422330</v>
@@ -7816,7 +7787,7 @@
     </row>
     <row r="50" spans="3:13" x14ac:dyDescent="0.4">
       <c r="C50" s="49" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D50" s="50">
         <v>187990</v>
@@ -7851,7 +7822,7 @@
     </row>
     <row r="51" spans="3:13" x14ac:dyDescent="0.4">
       <c r="C51" s="49" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D51" s="50">
         <v>169046</v>
@@ -7886,27 +7857,27 @@
     </row>
     <row r="53" spans="3:13" x14ac:dyDescent="0.4">
       <c r="D53" t="s">
+        <v>354</v>
+      </c>
+      <c r="E53" t="s">
         <v>355</v>
-      </c>
-      <c r="E53" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="54" spans="3:13" x14ac:dyDescent="0.4">
       <c r="E54" s="22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F54" s="33"/>
     </row>
     <row r="55" spans="3:13" x14ac:dyDescent="0.4">
       <c r="E55" s="22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F55" s="33"/>
     </row>
     <row r="56" spans="3:13" x14ac:dyDescent="0.4">
       <c r="E56" s="22" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F56" s="56"/>
     </row>
@@ -7956,13 +7927,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>302</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="C1" s="30" t="s">
         <v>303</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -17029,7 +17000,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="57" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -17037,7 +17008,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="57" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -17062,7 +17033,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574642DF-B6FC-47D7-8F4E-74F8116D6D0D}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -17307,12 +17278,13 @@
         <v>244</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B27" s="21"/>
       <c r="C27" s="21" t="s">
-        <v>426</v>
+        <v>289</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.4">
@@ -17327,91 +17299,72 @@
       </c>
       <c r="E30" s="9"/>
     </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="D31" s="22"/>
+      <c r="E31" s="1"/>
+    </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B32" s="21" t="s">
+      <c r="C32" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="D32" s="22"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B34" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="C32" s="21" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="D34" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="D35" s="22" t="s">
-        <v>287</v>
-      </c>
-      <c r="E35" s="9"/>
+      <c r="C34" s="21" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="D36" s="22"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C37" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="1"/>
+      <c r="C36" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="D38" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="E38" s="9"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B39" s="21" t="s">
+      <c r="D39" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="E39" s="9"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B41" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="C39" s="21" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C41" s="23" t="s">
-        <v>292</v>
+      <c r="C41" s="21" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="D43" s="22" t="s">
-        <v>293</v>
-      </c>
-      <c r="E43" s="9"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="D44" s="22" t="s">
-        <v>294</v>
-      </c>
-      <c r="E44" s="9"/>
+      <c r="C43" s="23" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="D45" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="E45" s="9"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B46" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C48" s="23" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D50" s="22" t="s">
+      <c r="D46" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="E50" s="9"/>
-    </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D51" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="E51" s="9"/>
+      <c r="E46" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -17435,10 +17388,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>407</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -17565,7 +17518,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B2" s="84" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.4">
@@ -17573,7 +17526,7 @@
         <v>70</v>
       </c>
       <c r="C3" s="86" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D3" s="85">
         <v>60</v>
@@ -17585,7 +17538,7 @@
     </row>
     <row r="6" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B6" s="84" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -17596,18 +17549,18 @@
     </row>
     <row r="9" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B9" s="89" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C9" s="89"/>
       <c r="D9" s="89" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E9" s="89"/>
       <c r="F9" s="89" t="s">
+        <v>410</v>
+      </c>
+      <c r="G9" s="89" t="s">
         <v>411</v>
-      </c>
-      <c r="G9" s="89" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -17621,10 +17574,10 @@
       </c>
       <c r="E10" s="90"/>
       <c r="F10" s="92" t="s">
+        <v>412</v>
+      </c>
+      <c r="G10" s="92" t="s">
         <v>413</v>
-      </c>
-      <c r="G10" s="92" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.4">
@@ -17644,13 +17597,13 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B13" s="84" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C13" s="84"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.4">
       <c r="C14" s="93" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
@@ -17659,10 +17612,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="95" t="s">
+        <v>361</v>
+      </c>
+      <c r="D16" s="96" t="s">
         <v>362</v>
-      </c>
-      <c r="D16" s="96" t="s">
-        <v>363</v>
       </c>
       <c r="F16" s="97"/>
     </row>
@@ -17786,7 +17739,7 @@
     </row>
     <row r="32" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B32" s="84" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -17794,10 +17747,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="95" t="s">
+        <v>361</v>
+      </c>
+      <c r="D33" s="96" t="s">
         <v>362</v>
-      </c>
-      <c r="D33" s="96" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="19.5" thickTop="1" x14ac:dyDescent="0.4">
@@ -17808,7 +17761,7 @@
         <v>67</v>
       </c>
       <c r="D34" s="100" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.4">
@@ -17819,7 +17772,7 @@
         <v>99</v>
       </c>
       <c r="D35" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.4">
@@ -17830,7 +17783,7 @@
         <v>75</v>
       </c>
       <c r="D36" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.4">
@@ -17841,7 +17794,7 @@
         <v>45</v>
       </c>
       <c r="D37" s="103" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.4">
@@ -17852,7 +17805,7 @@
         <v>55</v>
       </c>
       <c r="D38" s="103" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.4">
@@ -17863,7 +17816,7 @@
         <v>74</v>
       </c>
       <c r="D39" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.4">
@@ -17874,7 +17827,7 @@
         <v>67</v>
       </c>
       <c r="D40" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.4">
@@ -17885,7 +17838,7 @@
         <v>45</v>
       </c>
       <c r="D41" s="103" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.4">
@@ -17896,7 +17849,7 @@
         <v>70</v>
       </c>
       <c r="D42" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.4">
@@ -17907,7 +17860,7 @@
         <v>100</v>
       </c>
       <c r="D43" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.4">
@@ -17918,7 +17871,7 @@
         <v>66</v>
       </c>
       <c r="D44" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.4">
@@ -17929,7 +17882,7 @@
         <v>48</v>
       </c>
       <c r="D45" s="103" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -17940,7 +17893,7 @@
         <v>96</v>
       </c>
       <c r="D46" s="106" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -17966,13 +17919,13 @@
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B2" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B3" s="21"/>
       <c r="C3" s="72" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
@@ -17981,20 +17934,20 @@
         <v>1</v>
       </c>
       <c r="C5" s="70" t="s">
+        <v>361</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>366</v>
+      </c>
+      <c r="E5" s="71" t="s">
         <v>362</v>
       </c>
-      <c r="D5" s="76" t="s">
-        <v>367</v>
-      </c>
-      <c r="E5" s="71" t="s">
-        <v>363</v>
-      </c>
       <c r="G5" s="82" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H5" s="58"/>
       <c r="J5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="19.5" thickTop="1" x14ac:dyDescent="0.4">
@@ -18009,13 +17962,13 @@
       </c>
       <c r="E6" s="60"/>
       <c r="G6" s="22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H6" s="81">
         <v>60</v>
       </c>
       <c r="J6" s="80" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.4">
@@ -18030,13 +17983,13 @@
       </c>
       <c r="E7" s="62"/>
       <c r="G7" s="22" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H7" s="81">
         <v>60</v>
       </c>
       <c r="J7" s="80" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.4">
@@ -18173,7 +18126,7 @@
     </row>
     <row r="21" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="21" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -18181,13 +18134,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="70" t="s">
+        <v>361</v>
+      </c>
+      <c r="D22" s="76" t="s">
+        <v>366</v>
+      </c>
+      <c r="E22" s="71" t="s">
         <v>362</v>
-      </c>
-      <c r="D22" s="76" t="s">
-        <v>367</v>
-      </c>
-      <c r="E22" s="71" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4">
@@ -18201,7 +18154,7 @@
         <v>79</v>
       </c>
       <c r="E23" s="60" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.4">
@@ -18215,7 +18168,7 @@
         <v>62</v>
       </c>
       <c r="E24" s="62" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.4">
@@ -18229,7 +18182,7 @@
         <v>78</v>
       </c>
       <c r="E25" s="62" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.4">
@@ -18243,7 +18196,7 @@
         <v>58</v>
       </c>
       <c r="E26" s="62" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.4">
@@ -18257,7 +18210,7 @@
         <v>50</v>
       </c>
       <c r="E27" s="62" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.4">
@@ -18271,7 +18224,7 @@
         <v>70</v>
       </c>
       <c r="E28" s="62" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.4">
@@ -18285,7 +18238,7 @@
         <v>65</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.4">
@@ -18299,7 +18252,7 @@
         <v>44</v>
       </c>
       <c r="E30" s="62" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.4">
@@ -18313,7 +18266,7 @@
         <v>60</v>
       </c>
       <c r="E31" s="62" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.4">
@@ -18327,7 +18280,7 @@
         <v>80</v>
       </c>
       <c r="E32" s="62" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.4">
@@ -18341,7 +18294,7 @@
         <v>40</v>
       </c>
       <c r="E33" s="62" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.4">
@@ -18355,7 +18308,7 @@
         <v>35</v>
       </c>
       <c r="E34" s="62" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -18369,7 +18322,7 @@
         <v>85</v>
       </c>
       <c r="E35" s="64" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -18399,92 +18352,92 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="65"/>
       <c r="B2" s="65" t="s">
+        <v>368</v>
+      </c>
+      <c r="C2" s="65" t="s">
         <v>369</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="D2" s="65" t="s">
         <v>370</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="E2" s="65" t="s">
         <v>371</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="F2" s="65" t="s">
         <v>372</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="G2" s="65" t="s">
         <v>373</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="H2" s="65" t="s">
         <v>374</v>
       </c>
-      <c r="H2" s="65" t="s">
+      <c r="I2" s="65" t="s">
         <v>375</v>
       </c>
-      <c r="I2" s="65" t="s">
+      <c r="J2" s="65" t="s">
         <v>376</v>
-      </c>
-      <c r="J2" s="65" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="65" t="s">
+        <v>377</v>
+      </c>
+      <c r="B3" s="65" t="s">
         <v>378</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="C3" s="65" t="s">
         <v>379</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="D3" s="65" t="s">
         <v>380</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="E3" s="65" t="s">
         <v>381</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="F3" s="65" t="s">
         <v>382</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="G3" s="65" t="s">
         <v>383</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="H3" s="65" t="s">
         <v>384</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="I3" s="65" t="s">
         <v>385</v>
       </c>
-      <c r="I3" s="65" t="s">
+      <c r="J3" s="65" t="s">
         <v>386</v>
-      </c>
-      <c r="J3" s="65" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="65" t="s">
+        <v>387</v>
+      </c>
+      <c r="B4" s="65" t="s">
         <v>388</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="C4" s="65" t="s">
         <v>389</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="D4" s="65" t="s">
+        <v>383</v>
+      </c>
+      <c r="E4" s="65" t="s">
         <v>390</v>
       </c>
-      <c r="D4" s="65" t="s">
-        <v>384</v>
-      </c>
-      <c r="E4" s="65" t="s">
+      <c r="F4" s="65" t="s">
         <v>391</v>
       </c>
-      <c r="F4" s="65" t="s">
+      <c r="G4" s="65" t="s">
         <v>392</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>393</v>
       </c>
       <c r="H4" s="66"/>
       <c r="I4" s="66"/>
@@ -18492,103 +18445,103 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="65" t="s">
+        <v>393</v>
+      </c>
+      <c r="B5" s="65" t="s">
+        <v>388</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>391</v>
+      </c>
+      <c r="D5" s="25" t="s">
         <v>394</v>
       </c>
-      <c r="B5" s="65" t="s">
-        <v>389</v>
-      </c>
-      <c r="C5" s="65" t="s">
-        <v>392</v>
-      </c>
-      <c r="D5" s="25" t="s">
+      <c r="E5" s="65" t="s">
+        <v>384</v>
+      </c>
+      <c r="F5" s="65" t="s">
+        <v>380</v>
+      </c>
+      <c r="G5" s="65" t="s">
         <v>395</v>
       </c>
-      <c r="E5" s="65" t="s">
-        <v>385</v>
-      </c>
-      <c r="F5" s="65" t="s">
-        <v>381</v>
-      </c>
-      <c r="G5" s="65" t="s">
+      <c r="H5" s="65" t="s">
         <v>396</v>
       </c>
-      <c r="H5" s="65" t="s">
+      <c r="I5" s="65" t="s">
         <v>397</v>
-      </c>
-      <c r="I5" s="65" t="s">
-        <v>398</v>
       </c>
       <c r="J5" s="66"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="65" t="s">
+        <v>398</v>
+      </c>
+      <c r="B6" s="65" t="s">
         <v>399</v>
       </c>
-      <c r="B6" s="65" t="s">
-        <v>400</v>
-      </c>
       <c r="C6" s="65" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D6" s="65" t="s">
+        <v>385</v>
+      </c>
+      <c r="E6" s="65" t="s">
+        <v>389</v>
+      </c>
+      <c r="F6" s="65" t="s">
         <v>386</v>
       </c>
-      <c r="E6" s="65" t="s">
-        <v>390</v>
-      </c>
-      <c r="F6" s="65" t="s">
-        <v>387</v>
-      </c>
       <c r="G6" s="65" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H6" s="65" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I6" s="65" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J6" s="65" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="65" t="s">
+        <v>400</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>391</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>380</v>
+      </c>
+      <c r="D7" s="65" t="s">
         <v>401</v>
       </c>
-      <c r="B7" s="65" t="s">
-        <v>392</v>
-      </c>
-      <c r="C7" s="65" t="s">
-        <v>381</v>
-      </c>
-      <c r="D7" s="65" t="s">
+      <c r="E7" s="65" t="s">
+        <v>397</v>
+      </c>
+      <c r="F7" s="65" t="s">
+        <v>394</v>
+      </c>
+      <c r="G7" s="65" t="s">
+        <v>390</v>
+      </c>
+      <c r="H7" s="65" t="s">
         <v>402</v>
-      </c>
-      <c r="E7" s="65" t="s">
-        <v>398</v>
-      </c>
-      <c r="F7" s="65" t="s">
-        <v>395</v>
-      </c>
-      <c r="G7" s="65" t="s">
-        <v>391</v>
-      </c>
-      <c r="H7" s="65" t="s">
-        <v>403</v>
       </c>
       <c r="I7" s="66"/>
       <c r="J7" s="66"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B12" s="67" t="s">
+        <v>403</v>
+      </c>
+      <c r="C12" s="67" t="s">
         <v>404</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="D12" s="67" t="s">
         <v>405</v>
-      </c>
-      <c r="D12" s="67" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
change the only order of sheet
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://toyotajp-my.sharepoint.com/personal/3169885_tmc_twfr_toyota_co_jp/Documents/01_PA/04_人材育成/01_研修/01_デジタル全員研修/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="14_{2C160B8E-F762-48DE-84B6-0EB762DAF212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC18AC4A-9184-46CB-977D-40C3AA35B8BB}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="14_{2C160B8E-F762-48DE-84B6-0EB762DAF212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE274414-77CC-4DEB-B03E-13C68ADC492D}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="765" windowWidth="23625" windowHeight="14595" tabRatio="805" xr2:uid="{F6454EEB-C728-456F-9F74-DCB3B1160FD6}"/>
+    <workbookView xWindow="1530" yWindow="405" windowWidth="23925" windowHeight="14145" tabRatio="805" xr2:uid="{F6454EEB-C728-456F-9F74-DCB3B1160FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="基本" sheetId="3" r:id="rId1"/>
     <sheet name="関数" sheetId="2" r:id="rId2"/>
-    <sheet name="条件分岐" sheetId="12" r:id="rId3"/>
-    <sheet name="セル参照" sheetId="16" r:id="rId4"/>
-    <sheet name="条件付き書式" sheetId="17" r:id="rId5"/>
-    <sheet name="書式設定【基礎】" sheetId="6" r:id="rId6"/>
-    <sheet name="条件分岐（複数条件）" sheetId="13" r:id="rId7"/>
-    <sheet name="書式設定【応用】" sheetId="7" r:id="rId8"/>
-    <sheet name="関数【応用】" sheetId="10" r:id="rId9"/>
+    <sheet name="セル参照" sheetId="16" r:id="rId3"/>
+    <sheet name="条件付き書式" sheetId="17" r:id="rId4"/>
+    <sheet name="書式設定【基礎】" sheetId="6" r:id="rId5"/>
+    <sheet name="条件分岐（複数条件）" sheetId="13" r:id="rId6"/>
+    <sheet name="書式設定【応用】" sheetId="7" r:id="rId7"/>
+    <sheet name="関数【応用】" sheetId="10" r:id="rId8"/>
+    <sheet name="条件分岐" sheetId="12" r:id="rId9"/>
     <sheet name="ピボットテーブル" sheetId="18" r:id="rId10"/>
     <sheet name="TOYOTAカレンダー" sheetId="8" r:id="rId11"/>
     <sheet name="LIST" sheetId="11" state="hidden" r:id="rId12"/>
@@ -2999,9 +2999,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3012,6 +3009,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3299,6 +3299,346 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180388</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{846BB52B-8981-4511-8F53-1C8FFEB58A40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1890713" y="7634288"/>
+          <a:ext cx="366125" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>183563</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{223F5038-E341-4AB2-9036-968E0BFCCA82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1887538" y="10093325"/>
+          <a:ext cx="372475" cy="346075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>183563</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D9E8BD6-6415-433E-BEBE-62698221E60A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1887538" y="5373688"/>
+          <a:ext cx="372475" cy="346075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="377238" cy="374650"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="図 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{639CD6B9-E60C-4F78-8864-70E016BB3F0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1892300" y="6178550"/>
+          <a:ext cx="377238" cy="374650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="366126" cy="339725"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="図 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40470B20-26EB-4914-A4E1-861AC51269B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2000250" y="6400800"/>
+          <a:ext cx="366126" cy="339725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="366126" cy="346075"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E79C01B3-08D7-444D-B794-BE89EFADB79D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1695450" y="5083175"/>
+          <a:ext cx="366126" cy="346075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="366126" cy="342900"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F46986C-F6B0-4FFB-8AA4-BD027597149A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1695450" y="6196013"/>
+          <a:ext cx="366126" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3795,346 +4135,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>180388</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="図 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{846BB52B-8981-4511-8F53-1C8FFEB58A40}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1890713" y="7634288"/>
-          <a:ext cx="366125" cy="342900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>183563</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="図 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{223F5038-E341-4AB2-9036-968E0BFCCA82}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1887538" y="10093325"/>
-          <a:ext cx="372475" cy="346075"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>183563</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="図 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D9E8BD6-6415-433E-BEBE-62698221E60A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1887538" y="5373688"/>
-          <a:ext cx="372475" cy="346075"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="377238" cy="374650"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="図 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{639CD6B9-E60C-4F78-8864-70E016BB3F0C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1892300" y="6178550"/>
-          <a:ext cx="377238" cy="374650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="366126" cy="339725"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="図 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40470B20-26EB-4914-A4E1-861AC51269B3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2000250" y="6400800"/>
-          <a:ext cx="366126" cy="339725"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="366126" cy="346075"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="図 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E79C01B3-08D7-444D-B794-BE89EFADB79D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1695450" y="5083175"/>
-          <a:ext cx="366126" cy="346075"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="366126" cy="342900"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="図 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F46986C-F6B0-4FFB-8AA4-BD027597149A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1695450" y="6196013"/>
-          <a:ext cx="366126" cy="342900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
@@ -14460,362 +14460,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A632DF-1DFD-4A38-9700-AB7F101EBB78}">
-  <dimension ref="A1:G37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
-  <cols>
-    <col min="1" max="1" width="9" style="74"/>
-    <col min="2" max="2" width="11.5" style="74" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.625" style="74" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="74" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="74" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="74"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="75" t="s">
-        <v>177</v>
-      </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" s="75" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" s="75"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="B5" s="75"/>
-      <c r="C5" s="20" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="B6" s="75"/>
-      <c r="C6" s="20" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="19.5" thickBot="1">
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-    </row>
-    <row r="8" spans="1:7" ht="19.5" thickBot="1">
-      <c r="B8" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="78" t="s">
-        <v>150</v>
-      </c>
-      <c r="D8" s="79" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="19.5" thickTop="1">
-      <c r="B9" s="81" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="82">
-        <v>67</v>
-      </c>
-      <c r="D9" s="83"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="84" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="85">
-        <v>99</v>
-      </c>
-      <c r="D10" s="86"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" s="84" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="85">
-        <v>75</v>
-      </c>
-      <c r="D11" s="86"/>
-      <c r="F11" s="80"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" s="84" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="85">
-        <v>45</v>
-      </c>
-      <c r="D12" s="86"/>
-      <c r="F12" s="80"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13" s="84" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="85">
-        <v>55</v>
-      </c>
-      <c r="D13" s="86"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="84" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="85">
-        <v>74</v>
-      </c>
-      <c r="D14" s="86"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="84" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="85">
-        <v>67</v>
-      </c>
-      <c r="D15" s="86"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="84" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="85">
-        <v>45</v>
-      </c>
-      <c r="D16" s="86"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="85">
-        <v>70</v>
-      </c>
-      <c r="D17" s="86"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="84" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="85">
-        <v>100</v>
-      </c>
-      <c r="D18" s="86"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="85">
-        <v>66</v>
-      </c>
-      <c r="D19" s="86"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="84" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="85">
-        <v>48</v>
-      </c>
-      <c r="D20" s="86"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B21" s="87" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="88">
-        <v>96</v>
-      </c>
-      <c r="D21" s="89"/>
-    </row>
-    <row r="23" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B23" s="20" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B24" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="78" t="s">
-        <v>150</v>
-      </c>
-      <c r="D24" s="79" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" thickTop="1">
-      <c r="B25" s="81" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="82">
-        <v>67</v>
-      </c>
-      <c r="D25" s="83" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="84" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="85">
-        <v>99</v>
-      </c>
-      <c r="D26" s="86" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="84" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="85">
-        <v>75</v>
-      </c>
-      <c r="D27" s="86" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="84" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="85">
-        <v>45</v>
-      </c>
-      <c r="D28" s="86" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="84" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="85">
-        <v>55</v>
-      </c>
-      <c r="D29" s="86" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="84" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="85">
-        <v>74</v>
-      </c>
-      <c r="D30" s="86" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31" s="84" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="85">
-        <v>67</v>
-      </c>
-      <c r="D31" s="86" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="84" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="85">
-        <v>45</v>
-      </c>
-      <c r="D32" s="86" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="85">
-        <v>70</v>
-      </c>
-      <c r="D33" s="86" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="84" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="85">
-        <v>100</v>
-      </c>
-      <c r="D34" s="86" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4">
-      <c r="B35" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="85">
-        <v>66</v>
-      </c>
-      <c r="D35" s="86" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4">
-      <c r="B36" s="84" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="85">
-        <v>48</v>
-      </c>
-      <c r="D36" s="86" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="19.5" thickBot="1">
-      <c r="B37" s="87" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" s="88">
-        <v>96</v>
-      </c>
-      <c r="D37" s="89" t="s">
-        <v>152</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C87EC71-79C3-4E29-8E0E-17CCA82EC449}">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -14895,7 +14539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93646E48-9B96-4691-B9AF-F44A07EC392D}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -14959,7 +14603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0051BF1-256B-4B57-B5C2-7CB0BABD75BC}">
   <dimension ref="A1:AG50"/>
   <sheetViews>
@@ -15574,7 +15218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689EC7F3-02F8-430F-B583-4AFFA1276743}">
   <dimension ref="A1:J34"/>
   <sheetViews>
@@ -15999,7 +15643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C867672-5A85-4B0C-A0A5-E7FD6756FEBF}">
   <dimension ref="A1:BL29"/>
   <sheetViews>
@@ -16036,258 +15680,258 @@
       <c r="B5" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="117">
+      <c r="C5" s="116">
         <v>1</v>
       </c>
-      <c r="D5" s="118"/>
-      <c r="E5" s="117">
+      <c r="D5" s="117"/>
+      <c r="E5" s="116">
         <v>2</v>
       </c>
-      <c r="F5" s="118"/>
-      <c r="G5" s="117">
+      <c r="F5" s="117"/>
+      <c r="G5" s="116">
         <v>3</v>
       </c>
-      <c r="H5" s="118"/>
-      <c r="I5" s="117">
+      <c r="H5" s="117"/>
+      <c r="I5" s="116">
         <v>4</v>
       </c>
-      <c r="J5" s="118"/>
-      <c r="K5" s="119">
+      <c r="J5" s="117"/>
+      <c r="K5" s="118">
         <v>5</v>
       </c>
-      <c r="L5" s="120"/>
-      <c r="M5" s="119">
+      <c r="L5" s="119"/>
+      <c r="M5" s="118">
         <v>6</v>
       </c>
-      <c r="N5" s="120"/>
-      <c r="O5" s="117">
+      <c r="N5" s="119"/>
+      <c r="O5" s="116">
         <v>7</v>
       </c>
-      <c r="P5" s="118"/>
-      <c r="Q5" s="117">
+      <c r="P5" s="117"/>
+      <c r="Q5" s="116">
         <v>8</v>
       </c>
-      <c r="R5" s="118"/>
-      <c r="S5" s="117">
+      <c r="R5" s="117"/>
+      <c r="S5" s="116">
         <v>9</v>
       </c>
-      <c r="T5" s="118"/>
-      <c r="U5" s="117">
+      <c r="T5" s="117"/>
+      <c r="U5" s="116">
         <v>10</v>
       </c>
-      <c r="V5" s="118"/>
-      <c r="W5" s="117">
+      <c r="V5" s="117"/>
+      <c r="W5" s="116">
         <v>11</v>
       </c>
-      <c r="X5" s="118"/>
-      <c r="Y5" s="119">
+      <c r="X5" s="117"/>
+      <c r="Y5" s="118">
         <v>12</v>
       </c>
-      <c r="Z5" s="120"/>
-      <c r="AA5" s="119">
+      <c r="Z5" s="119"/>
+      <c r="AA5" s="118">
         <v>13</v>
       </c>
-      <c r="AB5" s="120"/>
-      <c r="AC5" s="117">
+      <c r="AB5" s="119"/>
+      <c r="AC5" s="116">
         <v>14</v>
       </c>
-      <c r="AD5" s="118"/>
-      <c r="AE5" s="117">
+      <c r="AD5" s="117"/>
+      <c r="AE5" s="116">
         <v>15</v>
       </c>
-      <c r="AF5" s="118"/>
-      <c r="AG5" s="117">
+      <c r="AF5" s="117"/>
+      <c r="AG5" s="116">
         <v>16</v>
       </c>
-      <c r="AH5" s="118"/>
-      <c r="AI5" s="117">
+      <c r="AH5" s="117"/>
+      <c r="AI5" s="116">
         <v>17</v>
       </c>
-      <c r="AJ5" s="118"/>
-      <c r="AK5" s="117">
+      <c r="AJ5" s="117"/>
+      <c r="AK5" s="116">
         <v>18</v>
       </c>
-      <c r="AL5" s="118"/>
-      <c r="AM5" s="119">
+      <c r="AL5" s="117"/>
+      <c r="AM5" s="118">
         <v>19</v>
       </c>
-      <c r="AN5" s="120"/>
-      <c r="AO5" s="119">
+      <c r="AN5" s="119"/>
+      <c r="AO5" s="118">
         <v>20</v>
       </c>
-      <c r="AP5" s="120"/>
-      <c r="AQ5" s="117">
+      <c r="AP5" s="119"/>
+      <c r="AQ5" s="116">
         <v>21</v>
       </c>
-      <c r="AR5" s="118"/>
-      <c r="AS5" s="117">
+      <c r="AR5" s="117"/>
+      <c r="AS5" s="116">
         <v>22</v>
       </c>
-      <c r="AT5" s="118"/>
-      <c r="AU5" s="117">
+      <c r="AT5" s="117"/>
+      <c r="AU5" s="116">
         <v>23</v>
       </c>
-      <c r="AV5" s="118"/>
-      <c r="AW5" s="117">
+      <c r="AV5" s="117"/>
+      <c r="AW5" s="116">
         <v>24</v>
       </c>
-      <c r="AX5" s="118"/>
-      <c r="AY5" s="117">
+      <c r="AX5" s="117"/>
+      <c r="AY5" s="116">
         <v>25</v>
       </c>
-      <c r="AZ5" s="118"/>
-      <c r="BA5" s="119">
+      <c r="AZ5" s="117"/>
+      <c r="BA5" s="118">
         <v>26</v>
       </c>
-      <c r="BB5" s="120"/>
-      <c r="BC5" s="119">
+      <c r="BB5" s="119"/>
+      <c r="BC5" s="118">
         <v>27</v>
       </c>
-      <c r="BD5" s="120"/>
-      <c r="BE5" s="117">
+      <c r="BD5" s="119"/>
+      <c r="BE5" s="116">
         <v>28</v>
       </c>
-      <c r="BF5" s="118"/>
-      <c r="BG5" s="117">
+      <c r="BF5" s="117"/>
+      <c r="BG5" s="116">
         <v>29</v>
       </c>
-      <c r="BH5" s="118"/>
-      <c r="BI5" s="117">
+      <c r="BH5" s="117"/>
+      <c r="BI5" s="116">
         <v>30</v>
       </c>
-      <c r="BJ5" s="118"/>
-      <c r="BK5" s="117">
+      <c r="BJ5" s="117"/>
+      <c r="BK5" s="116">
         <v>31</v>
       </c>
-      <c r="BL5" s="118"/>
+      <c r="BL5" s="117"/>
     </row>
     <row r="6" spans="1:64">
-      <c r="A6" s="116"/>
-      <c r="B6" s="116"/>
-      <c r="C6" s="117" t="s">
+      <c r="A6" s="120"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="118"/>
-      <c r="E6" s="117" t="s">
+      <c r="D6" s="117"/>
+      <c r="E6" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="118"/>
-      <c r="G6" s="117" t="s">
+      <c r="F6" s="117"/>
+      <c r="G6" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="118"/>
-      <c r="I6" s="117" t="s">
+      <c r="H6" s="117"/>
+      <c r="I6" s="116" t="s">
         <v>68</v>
       </c>
-      <c r="J6" s="118"/>
-      <c r="K6" s="119" t="s">
+      <c r="J6" s="117"/>
+      <c r="K6" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="L6" s="120"/>
-      <c r="M6" s="119" t="s">
+      <c r="L6" s="119"/>
+      <c r="M6" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="120"/>
-      <c r="O6" s="117" t="s">
+      <c r="N6" s="119"/>
+      <c r="O6" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="118"/>
-      <c r="Q6" s="117" t="s">
+      <c r="P6" s="117"/>
+      <c r="Q6" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="R6" s="118"/>
-      <c r="S6" s="117" t="s">
+      <c r="R6" s="117"/>
+      <c r="S6" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="T6" s="118"/>
-      <c r="U6" s="117" t="s">
+      <c r="T6" s="117"/>
+      <c r="U6" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="V6" s="118"/>
-      <c r="W6" s="117" t="s">
+      <c r="V6" s="117"/>
+      <c r="W6" s="116" t="s">
         <v>68</v>
       </c>
-      <c r="X6" s="118"/>
-      <c r="Y6" s="119" t="s">
+      <c r="X6" s="117"/>
+      <c r="Y6" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="Z6" s="120"/>
-      <c r="AA6" s="119" t="s">
+      <c r="Z6" s="119"/>
+      <c r="AA6" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="AB6" s="120"/>
-      <c r="AC6" s="117" t="s">
+      <c r="AB6" s="119"/>
+      <c r="AC6" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="AD6" s="118"/>
-      <c r="AE6" s="117" t="s">
+      <c r="AD6" s="117"/>
+      <c r="AE6" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="AF6" s="118"/>
-      <c r="AG6" s="117" t="s">
+      <c r="AF6" s="117"/>
+      <c r="AG6" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="AH6" s="118"/>
-      <c r="AI6" s="117" t="s">
+      <c r="AH6" s="117"/>
+      <c r="AI6" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="AJ6" s="118"/>
-      <c r="AK6" s="117" t="s">
+      <c r="AJ6" s="117"/>
+      <c r="AK6" s="116" t="s">
         <v>68</v>
       </c>
-      <c r="AL6" s="118"/>
-      <c r="AM6" s="119" t="s">
+      <c r="AL6" s="117"/>
+      <c r="AM6" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="AN6" s="120"/>
-      <c r="AO6" s="119" t="s">
+      <c r="AN6" s="119"/>
+      <c r="AO6" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="AP6" s="120"/>
-      <c r="AQ6" s="117" t="s">
+      <c r="AP6" s="119"/>
+      <c r="AQ6" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="AR6" s="118"/>
-      <c r="AS6" s="117" t="s">
+      <c r="AR6" s="117"/>
+      <c r="AS6" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="AT6" s="118"/>
-      <c r="AU6" s="117" t="s">
+      <c r="AT6" s="117"/>
+      <c r="AU6" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="AV6" s="118"/>
-      <c r="AW6" s="117" t="s">
+      <c r="AV6" s="117"/>
+      <c r="AW6" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="AX6" s="118"/>
-      <c r="AY6" s="117" t="s">
+      <c r="AX6" s="117"/>
+      <c r="AY6" s="116" t="s">
         <v>68</v>
       </c>
-      <c r="AZ6" s="118"/>
-      <c r="BA6" s="119" t="s">
+      <c r="AZ6" s="117"/>
+      <c r="BA6" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="BB6" s="120"/>
-      <c r="BC6" s="119" t="s">
+      <c r="BB6" s="119"/>
+      <c r="BC6" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="BD6" s="120"/>
-      <c r="BE6" s="117" t="s">
+      <c r="BD6" s="119"/>
+      <c r="BE6" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="BF6" s="118"/>
-      <c r="BG6" s="117" t="s">
+      <c r="BF6" s="117"/>
+      <c r="BG6" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="BH6" s="118"/>
-      <c r="BI6" s="117" t="s">
+      <c r="BH6" s="117"/>
+      <c r="BI6" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="BJ6" s="118"/>
-      <c r="BK6" s="117" t="s">
+      <c r="BJ6" s="117"/>
+      <c r="BK6" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="BL6" s="118"/>
+      <c r="BL6" s="117"/>
     </row>
     <row r="7" spans="1:64">
       <c r="A7" s="115"/>
@@ -16807,54 +16451,6 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="BE6:BF6"/>
-    <mergeCell ref="BG6:BH6"/>
-    <mergeCell ref="BI6:BJ6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="BA6:BB6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BG5:BH5"/>
-    <mergeCell ref="BI5:BJ5"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BE5:BF5"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="AS6:AT6"/>
@@ -16871,6 +16467,54 @@
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="BG5:BH5"/>
+    <mergeCell ref="BI5:BJ5"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BE5:BF5"/>
+    <mergeCell ref="BE6:BF6"/>
+    <mergeCell ref="BG6:BH6"/>
+    <mergeCell ref="BI6:BJ6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="BA6:BB6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AS5:AT5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16878,7 +16522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D41923-D28C-4D44-B8F8-AD674F8993FB}">
   <dimension ref="B2:O56"/>
   <sheetViews>
@@ -17515,4 +17159,360 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A632DF-1DFD-4A38-9700-AB7F101EBB78}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="1" width="9" style="74"/>
+    <col min="2" max="2" width="11.5" style="74" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.625" style="74" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="74" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.375" style="74" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="74"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="75" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="75" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="75"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" s="75"/>
+      <c r="C5" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" s="75"/>
+      <c r="C6" s="20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="19.5" thickBot="1">
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+    </row>
+    <row r="8" spans="1:7" ht="19.5" thickBot="1">
+      <c r="B8" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="78" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="79" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="19.5" thickTop="1">
+      <c r="B9" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="82">
+        <v>67</v>
+      </c>
+      <c r="D9" s="83"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="85">
+        <v>99</v>
+      </c>
+      <c r="D10" s="86"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="84" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="85">
+        <v>75</v>
+      </c>
+      <c r="D11" s="86"/>
+      <c r="F11" s="80"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="85">
+        <v>45</v>
+      </c>
+      <c r="D12" s="86"/>
+      <c r="F12" s="80"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="85">
+        <v>55</v>
+      </c>
+      <c r="D13" s="86"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="85">
+        <v>74</v>
+      </c>
+      <c r="D14" s="86"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="85">
+        <v>67</v>
+      </c>
+      <c r="D15" s="86"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="85">
+        <v>45</v>
+      </c>
+      <c r="D16" s="86"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="85">
+        <v>70</v>
+      </c>
+      <c r="D17" s="86"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="84" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="85">
+        <v>100</v>
+      </c>
+      <c r="D18" s="86"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="85">
+        <v>66</v>
+      </c>
+      <c r="D19" s="86"/>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="84" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="85">
+        <v>48</v>
+      </c>
+      <c r="D20" s="86"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B21" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="88">
+        <v>96</v>
+      </c>
+      <c r="D21" s="89"/>
+    </row>
+    <row r="23" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B23" s="20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B24" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="78" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" s="79" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" thickTop="1">
+      <c r="B25" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="82">
+        <v>67</v>
+      </c>
+      <c r="D25" s="83" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="85">
+        <v>99</v>
+      </c>
+      <c r="D26" s="86" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="84" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="85">
+        <v>75</v>
+      </c>
+      <c r="D27" s="86" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="85">
+        <v>45</v>
+      </c>
+      <c r="D28" s="86" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="85">
+        <v>55</v>
+      </c>
+      <c r="D29" s="86" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="85">
+        <v>74</v>
+      </c>
+      <c r="D30" s="86" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="85">
+        <v>67</v>
+      </c>
+      <c r="D31" s="86" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="85">
+        <v>45</v>
+      </c>
+      <c r="D32" s="86" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="85">
+        <v>70</v>
+      </c>
+      <c r="D33" s="86" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="84" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="85">
+        <v>100</v>
+      </c>
+      <c r="D34" s="86" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="85">
+        <v>66</v>
+      </c>
+      <c r="D35" s="86" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="84" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="85">
+        <v>48</v>
+      </c>
+      <c r="D36" s="86" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B37" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="88">
+        <v>96</v>
+      </c>
+      <c r="D37" s="89" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change the hint of function
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://toyotajp-my.sharepoint.com/personal/3169885_tmc_twfr_toyota_co_jp/Documents/01_PA/04_人材育成/01_研修/01_デジタル全員研修/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="14_{2C160B8E-F762-48DE-84B6-0EB762DAF212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE274414-77CC-4DEB-B03E-13C68ADC492D}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="14_{2C160B8E-F762-48DE-84B6-0EB762DAF212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3585AC50-2278-402C-A43B-CA759D5E288A}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="405" windowWidth="23925" windowHeight="14145" tabRatio="805" xr2:uid="{F6454EEB-C728-456F-9F74-DCB3B1160FD6}"/>
+    <workbookView xWindow="1260" yWindow="405" windowWidth="23415" windowHeight="14325" tabRatio="805" xr2:uid="{F6454EEB-C728-456F-9F74-DCB3B1160FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="基本" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="233">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -1581,40 +1581,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>表の「姓」「名」それぞれの列に、「氏名」列から関数で取得した値を表示してください</t>
-    <rPh sb="0" eb="1">
-      <t>ヒョウ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>セイ</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>レツ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>シメイ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>レツ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>カンスウ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>シュトク</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>アタイ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>文字列操作関数の問題です。</t>
     <rPh sb="0" eb="5">
       <t>モジレツソウサ</t>
@@ -2032,6 +1998,78 @@
     <t>チャレンジ演習！</t>
     <rPh sb="5" eb="7">
       <t>エンシュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>性別が女性のセルだけを選択するようなこともできますが、</t>
+    <rPh sb="0" eb="2">
+      <t>セイベツ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジョセイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>これが5レコードだけではなく5,000レコードあったら疲れますよね？</t>
+    <rPh sb="27" eb="28">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>もっと良いやり方があるかもしれません</t>
+    <rPh sb="3" eb="4">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>表の「姓」「名」それぞれの列（I4、J4からのセル）に表示してください</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「氏名」列（B4からのセル）から「姓」と「名」を関数で取得して、</t>
+    <rPh sb="17" eb="18">
+      <t>セイ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>カンスウ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（文字数を直接数値で指定すると、八木澤さんや坂口さんは？？？）</t>
+    <rPh sb="1" eb="4">
+      <t>モジスウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>チョクセツ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>スウチ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="16" eb="19">
+      <t>ヤギサワ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>サカグチ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2639,7 +2677,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2999,6 +3037,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3011,8 +3052,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3154,13 +3195,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>338138</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>712518</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>21272</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3254,7 +3295,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>338138</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="374380" cy="378460"/>
@@ -4532,40 +4573,40 @@
         <v>43</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="104" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="105" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="B6" s="105" t="s">
+      <c r="C6" s="106" t="s">
         <v>200</v>
       </c>
-      <c r="C6" s="106" t="s">
+      <c r="D6" s="107" t="s">
         <v>201</v>
       </c>
-      <c r="D6" s="107" t="s">
+      <c r="E6" s="107" t="s">
         <v>202</v>
       </c>
-      <c r="E6" s="107" t="s">
+      <c r="F6" s="107" t="s">
         <v>203</v>
       </c>
-      <c r="F6" s="107" t="s">
+      <c r="G6" s="107" t="s">
         <v>204</v>
-      </c>
-      <c r="G6" s="107" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4573,10 +4614,10 @@
         <v>45677</v>
       </c>
       <c r="B7" s="109" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="109" t="s">
         <v>206</v>
-      </c>
-      <c r="C7" s="109" t="s">
-        <v>207</v>
       </c>
       <c r="D7" s="110">
         <v>12000</v>
@@ -4598,10 +4639,10 @@
         <v>45698</v>
       </c>
       <c r="B8" s="109" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" s="109" t="s">
         <v>208</v>
-      </c>
-      <c r="C8" s="109" t="s">
-        <v>209</v>
       </c>
       <c r="D8" s="110">
         <v>9000</v>
@@ -4623,10 +4664,10 @@
         <v>45698</v>
       </c>
       <c r="B9" s="109" t="s">
+        <v>209</v>
+      </c>
+      <c r="C9" s="109" t="s">
         <v>210</v>
-      </c>
-      <c r="C9" s="109" t="s">
-        <v>211</v>
       </c>
       <c r="D9" s="110">
         <v>7000</v>
@@ -4648,10 +4689,10 @@
         <v>45718</v>
       </c>
       <c r="B10" s="109" t="s">
+        <v>211</v>
+      </c>
+      <c r="C10" s="109" t="s">
         <v>212</v>
-      </c>
-      <c r="C10" s="109" t="s">
-        <v>213</v>
       </c>
       <c r="D10" s="110">
         <v>10000</v>
@@ -4673,10 +4714,10 @@
         <v>45727</v>
       </c>
       <c r="B11" s="109" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" s="109" t="s">
         <v>206</v>
-      </c>
-      <c r="C11" s="109" t="s">
-        <v>207</v>
       </c>
       <c r="D11" s="110">
         <v>12000</v>
@@ -4698,10 +4739,10 @@
         <v>45768</v>
       </c>
       <c r="B12" s="109" t="s">
+        <v>213</v>
+      </c>
+      <c r="C12" s="109" t="s">
         <v>214</v>
-      </c>
-      <c r="C12" s="109" t="s">
-        <v>215</v>
       </c>
       <c r="D12" s="110">
         <v>6000</v>
@@ -4723,10 +4764,10 @@
         <v>45768</v>
       </c>
       <c r="B13" s="109" t="s">
+        <v>215</v>
+      </c>
+      <c r="C13" s="109" t="s">
         <v>216</v>
-      </c>
-      <c r="C13" s="109" t="s">
-        <v>217</v>
       </c>
       <c r="D13" s="110">
         <v>16000</v>
@@ -4748,10 +4789,10 @@
         <v>45793</v>
       </c>
       <c r="B14" s="109" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" s="109" t="s">
         <v>206</v>
-      </c>
-      <c r="C14" s="109" t="s">
-        <v>207</v>
       </c>
       <c r="D14" s="110">
         <v>12000</v>
@@ -4773,10 +4814,10 @@
         <v>45793</v>
       </c>
       <c r="B15" s="109" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15" s="109" t="s">
         <v>208</v>
-      </c>
-      <c r="C15" s="109" t="s">
-        <v>209</v>
       </c>
       <c r="D15" s="110">
         <v>9000</v>
@@ -4798,10 +4839,10 @@
         <v>45809</v>
       </c>
       <c r="B16" s="109" t="s">
+        <v>217</v>
+      </c>
+      <c r="C16" s="109" t="s">
         <v>218</v>
-      </c>
-      <c r="C16" s="109" t="s">
-        <v>219</v>
       </c>
       <c r="D16" s="110">
         <v>10000</v>
@@ -4823,10 +4864,10 @@
         <v>45826</v>
       </c>
       <c r="B17" s="109" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" s="109" t="s">
         <v>214</v>
-      </c>
-      <c r="C17" s="109" t="s">
-        <v>215</v>
       </c>
       <c r="D17" s="110">
         <v>6000</v>
@@ -14109,7 +14150,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574642DF-B6FC-47D7-8F4E-74F8116D6D0D}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -14281,7 +14322,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>14</v>
@@ -14415,41 +14456,72 @@
       </c>
       <c r="E35" s="9"/>
     </row>
+    <row r="36" spans="2:5">
+      <c r="D36" s="19"/>
+      <c r="E36" s="121"/>
+    </row>
     <row r="37" spans="2:5">
       <c r="C37" s="20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="C38" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="C39" s="20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="C40" s="20" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="18" t="s">
+    <row r="42" spans="2:5">
+      <c r="B42" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C42" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" s="18"/>
+      <c r="C43" s="18" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" s="18"/>
+      <c r="C44" s="18" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="D45" s="19"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="C46" s="20" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="C47" s="20" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="2:5">
-      <c r="C40" s="18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5">
-      <c r="D41" s="19"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="C42" s="20" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5">
-      <c r="C43" s="20" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5">
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
+    <row r="48" spans="2:5">
+      <c r="C48" s="20" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -14557,7 +14629,7 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F3" s="5"/>
     </row>
@@ -14570,11 +14642,11 @@
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -14585,12 +14657,12 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -15019,20 +15091,20 @@
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:33">
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:33">
       <c r="B16" s="18"/>
       <c r="D16" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="2:5">
@@ -15044,7 +15116,7 @@
         <v>46</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="2:5">
@@ -15073,7 +15145,7 @@
         <v>46</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="2:5">
@@ -15115,7 +15187,7 @@
     <row r="34" spans="3:22">
       <c r="C34" s="18"/>
       <c r="D34" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="3:22">
@@ -15123,7 +15195,7 @@
         <v>46</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T36" s="19"/>
       <c r="U36" s="20"/>
@@ -15131,7 +15203,7 @@
     <row r="37" spans="3:22">
       <c r="D37" s="19"/>
       <c r="F37" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T37" s="19"/>
       <c r="U37" s="20"/>
@@ -15139,7 +15211,7 @@
     <row r="38" spans="3:22">
       <c r="D38" s="19"/>
       <c r="F38" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T38" s="19"/>
       <c r="U38" s="20"/>
@@ -15157,19 +15229,19 @@
         <v>46</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T40" s="19"/>
       <c r="U40" s="20"/>
     </row>
     <row r="41" spans="3:22">
       <c r="F41" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="3:22">
       <c r="F42" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="3:22">
@@ -15180,7 +15252,7 @@
     </row>
     <row r="45" spans="3:22">
       <c r="C45" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D45" s="18"/>
     </row>
@@ -15201,7 +15273,7 @@
         <v>46</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="4:5">
@@ -15680,258 +15752,258 @@
       <c r="B5" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="116">
+      <c r="C5" s="117">
         <v>1</v>
       </c>
-      <c r="D5" s="117"/>
-      <c r="E5" s="116">
+      <c r="D5" s="118"/>
+      <c r="E5" s="117">
         <v>2</v>
       </c>
-      <c r="F5" s="117"/>
-      <c r="G5" s="116">
+      <c r="F5" s="118"/>
+      <c r="G5" s="117">
         <v>3</v>
       </c>
-      <c r="H5" s="117"/>
-      <c r="I5" s="116">
+      <c r="H5" s="118"/>
+      <c r="I5" s="117">
         <v>4</v>
       </c>
-      <c r="J5" s="117"/>
-      <c r="K5" s="118">
+      <c r="J5" s="118"/>
+      <c r="K5" s="119">
         <v>5</v>
       </c>
-      <c r="L5" s="119"/>
-      <c r="M5" s="118">
+      <c r="L5" s="120"/>
+      <c r="M5" s="119">
         <v>6</v>
       </c>
-      <c r="N5" s="119"/>
-      <c r="O5" s="116">
+      <c r="N5" s="120"/>
+      <c r="O5" s="117">
         <v>7</v>
       </c>
-      <c r="P5" s="117"/>
-      <c r="Q5" s="116">
+      <c r="P5" s="118"/>
+      <c r="Q5" s="117">
         <v>8</v>
       </c>
-      <c r="R5" s="117"/>
-      <c r="S5" s="116">
+      <c r="R5" s="118"/>
+      <c r="S5" s="117">
         <v>9</v>
       </c>
-      <c r="T5" s="117"/>
-      <c r="U5" s="116">
+      <c r="T5" s="118"/>
+      <c r="U5" s="117">
         <v>10</v>
       </c>
-      <c r="V5" s="117"/>
-      <c r="W5" s="116">
+      <c r="V5" s="118"/>
+      <c r="W5" s="117">
         <v>11</v>
       </c>
-      <c r="X5" s="117"/>
-      <c r="Y5" s="118">
+      <c r="X5" s="118"/>
+      <c r="Y5" s="119">
         <v>12</v>
       </c>
-      <c r="Z5" s="119"/>
-      <c r="AA5" s="118">
+      <c r="Z5" s="120"/>
+      <c r="AA5" s="119">
         <v>13</v>
       </c>
-      <c r="AB5" s="119"/>
-      <c r="AC5" s="116">
+      <c r="AB5" s="120"/>
+      <c r="AC5" s="117">
         <v>14</v>
       </c>
-      <c r="AD5" s="117"/>
-      <c r="AE5" s="116">
+      <c r="AD5" s="118"/>
+      <c r="AE5" s="117">
         <v>15</v>
       </c>
-      <c r="AF5" s="117"/>
-      <c r="AG5" s="116">
+      <c r="AF5" s="118"/>
+      <c r="AG5" s="117">
         <v>16</v>
       </c>
-      <c r="AH5" s="117"/>
-      <c r="AI5" s="116">
+      <c r="AH5" s="118"/>
+      <c r="AI5" s="117">
         <v>17</v>
       </c>
-      <c r="AJ5" s="117"/>
-      <c r="AK5" s="116">
+      <c r="AJ5" s="118"/>
+      <c r="AK5" s="117">
         <v>18</v>
       </c>
-      <c r="AL5" s="117"/>
-      <c r="AM5" s="118">
+      <c r="AL5" s="118"/>
+      <c r="AM5" s="119">
         <v>19</v>
       </c>
-      <c r="AN5" s="119"/>
-      <c r="AO5" s="118">
+      <c r="AN5" s="120"/>
+      <c r="AO5" s="119">
         <v>20</v>
       </c>
-      <c r="AP5" s="119"/>
-      <c r="AQ5" s="116">
+      <c r="AP5" s="120"/>
+      <c r="AQ5" s="117">
         <v>21</v>
       </c>
-      <c r="AR5" s="117"/>
-      <c r="AS5" s="116">
+      <c r="AR5" s="118"/>
+      <c r="AS5" s="117">
         <v>22</v>
       </c>
-      <c r="AT5" s="117"/>
-      <c r="AU5" s="116">
+      <c r="AT5" s="118"/>
+      <c r="AU5" s="117">
         <v>23</v>
       </c>
-      <c r="AV5" s="117"/>
-      <c r="AW5" s="116">
+      <c r="AV5" s="118"/>
+      <c r="AW5" s="117">
         <v>24</v>
       </c>
-      <c r="AX5" s="117"/>
-      <c r="AY5" s="116">
+      <c r="AX5" s="118"/>
+      <c r="AY5" s="117">
         <v>25</v>
       </c>
-      <c r="AZ5" s="117"/>
-      <c r="BA5" s="118">
+      <c r="AZ5" s="118"/>
+      <c r="BA5" s="119">
         <v>26</v>
       </c>
-      <c r="BB5" s="119"/>
-      <c r="BC5" s="118">
+      <c r="BB5" s="120"/>
+      <c r="BC5" s="119">
         <v>27</v>
       </c>
-      <c r="BD5" s="119"/>
-      <c r="BE5" s="116">
+      <c r="BD5" s="120"/>
+      <c r="BE5" s="117">
         <v>28</v>
       </c>
-      <c r="BF5" s="117"/>
-      <c r="BG5" s="116">
+      <c r="BF5" s="118"/>
+      <c r="BG5" s="117">
         <v>29</v>
       </c>
-      <c r="BH5" s="117"/>
-      <c r="BI5" s="116">
+      <c r="BH5" s="118"/>
+      <c r="BI5" s="117">
         <v>30</v>
       </c>
-      <c r="BJ5" s="117"/>
-      <c r="BK5" s="116">
+      <c r="BJ5" s="118"/>
+      <c r="BK5" s="117">
         <v>31</v>
       </c>
-      <c r="BL5" s="117"/>
+      <c r="BL5" s="118"/>
     </row>
     <row r="6" spans="1:64">
-      <c r="A6" s="120"/>
-      <c r="B6" s="120"/>
-      <c r="C6" s="116" t="s">
+      <c r="A6" s="116"/>
+      <c r="B6" s="116"/>
+      <c r="C6" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="117"/>
-      <c r="E6" s="116" t="s">
+      <c r="D6" s="118"/>
+      <c r="E6" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="117"/>
-      <c r="G6" s="116" t="s">
+      <c r="F6" s="118"/>
+      <c r="G6" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="117"/>
-      <c r="I6" s="116" t="s">
+      <c r="H6" s="118"/>
+      <c r="I6" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="J6" s="117"/>
-      <c r="K6" s="118" t="s">
+      <c r="J6" s="118"/>
+      <c r="K6" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="L6" s="119"/>
-      <c r="M6" s="118" t="s">
+      <c r="L6" s="120"/>
+      <c r="M6" s="119" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="119"/>
-      <c r="O6" s="116" t="s">
+      <c r="N6" s="120"/>
+      <c r="O6" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="117"/>
-      <c r="Q6" s="116" t="s">
+      <c r="P6" s="118"/>
+      <c r="Q6" s="117" t="s">
         <v>64</v>
       </c>
-      <c r="R6" s="117"/>
-      <c r="S6" s="116" t="s">
+      <c r="R6" s="118"/>
+      <c r="S6" s="117" t="s">
         <v>63</v>
       </c>
-      <c r="T6" s="117"/>
-      <c r="U6" s="116" t="s">
+      <c r="T6" s="118"/>
+      <c r="U6" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="V6" s="117"/>
-      <c r="W6" s="116" t="s">
+      <c r="V6" s="118"/>
+      <c r="W6" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="X6" s="117"/>
-      <c r="Y6" s="118" t="s">
+      <c r="X6" s="118"/>
+      <c r="Y6" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="Z6" s="119"/>
-      <c r="AA6" s="118" t="s">
+      <c r="Z6" s="120"/>
+      <c r="AA6" s="119" t="s">
         <v>66</v>
       </c>
-      <c r="AB6" s="119"/>
-      <c r="AC6" s="116" t="s">
+      <c r="AB6" s="120"/>
+      <c r="AC6" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="AD6" s="117"/>
-      <c r="AE6" s="116" t="s">
+      <c r="AD6" s="118"/>
+      <c r="AE6" s="117" t="s">
         <v>64</v>
       </c>
-      <c r="AF6" s="117"/>
-      <c r="AG6" s="116" t="s">
+      <c r="AF6" s="118"/>
+      <c r="AG6" s="117" t="s">
         <v>63</v>
       </c>
-      <c r="AH6" s="117"/>
-      <c r="AI6" s="116" t="s">
+      <c r="AH6" s="118"/>
+      <c r="AI6" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="AJ6" s="117"/>
-      <c r="AK6" s="116" t="s">
+      <c r="AJ6" s="118"/>
+      <c r="AK6" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="AL6" s="117"/>
-      <c r="AM6" s="118" t="s">
+      <c r="AL6" s="118"/>
+      <c r="AM6" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="AN6" s="119"/>
-      <c r="AO6" s="118" t="s">
+      <c r="AN6" s="120"/>
+      <c r="AO6" s="119" t="s">
         <v>66</v>
       </c>
-      <c r="AP6" s="119"/>
-      <c r="AQ6" s="116" t="s">
+      <c r="AP6" s="120"/>
+      <c r="AQ6" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="AR6" s="117"/>
-      <c r="AS6" s="116" t="s">
+      <c r="AR6" s="118"/>
+      <c r="AS6" s="117" t="s">
         <v>64</v>
       </c>
-      <c r="AT6" s="117"/>
-      <c r="AU6" s="116" t="s">
+      <c r="AT6" s="118"/>
+      <c r="AU6" s="117" t="s">
         <v>63</v>
       </c>
-      <c r="AV6" s="117"/>
-      <c r="AW6" s="116" t="s">
+      <c r="AV6" s="118"/>
+      <c r="AW6" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="AX6" s="117"/>
-      <c r="AY6" s="116" t="s">
+      <c r="AX6" s="118"/>
+      <c r="AY6" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="AZ6" s="117"/>
-      <c r="BA6" s="118" t="s">
+      <c r="AZ6" s="118"/>
+      <c r="BA6" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="BB6" s="119"/>
-      <c r="BC6" s="118" t="s">
+      <c r="BB6" s="120"/>
+      <c r="BC6" s="119" t="s">
         <v>66</v>
       </c>
-      <c r="BD6" s="119"/>
-      <c r="BE6" s="116" t="s">
+      <c r="BD6" s="120"/>
+      <c r="BE6" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="BF6" s="117"/>
-      <c r="BG6" s="116" t="s">
+      <c r="BF6" s="118"/>
+      <c r="BG6" s="117" t="s">
         <v>64</v>
       </c>
-      <c r="BH6" s="117"/>
-      <c r="BI6" s="116" t="s">
+      <c r="BH6" s="118"/>
+      <c r="BI6" s="117" t="s">
         <v>63</v>
       </c>
-      <c r="BJ6" s="117"/>
-      <c r="BK6" s="116" t="s">
+      <c r="BJ6" s="118"/>
+      <c r="BK6" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="BL6" s="117"/>
+      <c r="BL6" s="118"/>
     </row>
     <row r="7" spans="1:64">
       <c r="A7" s="115"/>
@@ -16451,6 +16523,54 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AS5:AT5"/>
+    <mergeCell ref="BE6:BF6"/>
+    <mergeCell ref="BG6:BH6"/>
+    <mergeCell ref="BI6:BJ6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="BA6:BB6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BG5:BH5"/>
+    <mergeCell ref="BI5:BJ5"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BE5:BF5"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="AS6:AT6"/>
@@ -16467,54 +16587,6 @@
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="BG5:BH5"/>
-    <mergeCell ref="BI5:BJ5"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BE5:BF5"/>
-    <mergeCell ref="BE6:BF6"/>
-    <mergeCell ref="BG6:BH6"/>
-    <mergeCell ref="BI6:BJ6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="BA6:BB6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>